<commit_message>
Pequenos ajustes e correcoes v2
</commit_message>
<xml_diff>
--- a/LOGIN-PAINEL/logs_acesso.xlsx
+++ b/LOGIN-PAINEL/logs_acesso.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://giroprodutos-my.sharepoint.com/personal/cig360_giroprodutos_onmicrosoft_com/Documents/COMPARTILHADA - CIG360/02_RELATORIOS/09_PYTHON/LOGIN-PAINEL/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_45B940EFF613C8264D4E48C325B0FDBA7452F358" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5DF815D-D0C6-4F39-B1FB-C8D38B2AF801}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
   <si>
     <t>data_login</t>
   </si>
@@ -104,6 +98,15 @@
   </si>
   <si>
     <t>16:32:01</t>
+  </si>
+  <si>
+    <t>17:02:50</t>
+  </si>
+  <si>
+    <t>17:07:19</t>
+  </si>
+  <si>
+    <t>17:07:36</t>
   </si>
   <si>
     <t>joao</t>
@@ -148,8 +151,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,21 +215,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -264,7 +259,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -298,7 +293,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -333,10 +327,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -509,25 +502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -561,25 +543,25 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -587,16 +569,16 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -604,16 +586,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -621,16 +603,16 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -638,25 +620,25 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -664,16 +646,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -681,16 +663,16 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -698,16 +680,16 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -715,16 +697,16 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -732,25 +714,25 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -758,25 +740,25 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -784,13 +766,13 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -798,13 +780,13 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -812,13 +794,13 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -826,13 +808,13 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -840,13 +822,13 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -854,13 +836,13 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -868,13 +850,13 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -882,10 +864,52 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="D20" t="s">
-        <v>31</v>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcao de caminhos dos arquivos para nuvem
</commit_message>
<xml_diff>
--- a/LOGIN-PAINEL/logs_acesso.xlsx
+++ b/LOGIN-PAINEL/logs_acesso.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="45">
   <si>
     <t>data_login</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>17:07:36</t>
+  </si>
+  <si>
+    <t>17:09:45</t>
   </si>
   <si>
     <t>joao</t>
@@ -503,7 +506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -543,22 +546,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -569,13 +572,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -586,13 +589,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -603,13 +606,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -620,22 +623,22 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -646,13 +649,13 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -663,13 +666,13 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -680,13 +683,13 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -697,13 +700,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -714,22 +717,22 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -740,22 +743,22 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -766,10 +769,10 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -780,10 +783,10 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -794,10 +797,10 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -808,10 +811,10 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -822,10 +825,10 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -836,10 +839,10 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -850,10 +853,10 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -864,10 +867,10 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -878,10 +881,10 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -892,10 +895,10 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -906,10 +909,24 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>